<commit_message>
FIxed Save Game Function #10
create a new txt file to save the data and included the turns and buildings left into the save function.
</commit_message>
<xml_diff>
--- a/data/save_board.xlsx
+++ b/data/save_board.xlsx
@@ -686,7 +686,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>SHP</t>
+          <t>FAC</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>HWY</t>
+          <t>FAC</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Commenting out minor print issue. #10
</commit_message>
<xml_diff>
--- a/data/save_board.xlsx
+++ b/data/save_board.xlsx
@@ -686,7 +686,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>FAC</t>
+          <t>SHP</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -711,17 +711,17 @@
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>n</t>
+          <t>e</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>FAC</t>
+          <t>e</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
-          <t>n</t>
+          <t>e</t>
         </is>
       </c>
       <c r="M3" s="1" t="inlineStr">
@@ -943,17 +943,17 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>FAC</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Fixed issues #5 #6 #7 #10 #12
</commit_message>
<xml_diff>
--- a/data/save_board.xlsx
+++ b/data/save_board.xlsx
@@ -681,47 +681,47 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
           <t>n</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>SHP</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>HSE</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
         <is>
           <t>n</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
         </is>
       </c>
       <c r="M3" s="1" t="inlineStr">
@@ -943,49 +943,49 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
           <t>n</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>FAC</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>HWY</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr">
         <is>
           <t>n</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
       <c r="M5" s="1" t="inlineStr">
         <is>
           <t>e</t>
@@ -1003,17 +1003,17 @@
       </c>
       <c r="P5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="Q5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>SHP</t>
         </is>
       </c>
       <c r="R5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="S5" s="1" t="inlineStr">
@@ -1033,17 +1033,17 @@
       </c>
       <c r="V5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="W5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>HSE</t>
         </is>
       </c>
       <c r="X5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="Y5" s="1" t="inlineStr">
@@ -1235,17 +1235,17 @@
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="M7" s="1" t="inlineStr">
@@ -1295,17 +1295,17 @@
       </c>
       <c r="V7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="W7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>FAC</t>
         </is>
       </c>
       <c r="X7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="Y7" s="1" t="inlineStr">
@@ -1557,17 +1557,17 @@
       </c>
       <c r="V9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="W9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="X9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="Y9" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Finished development for high score leaderboard #21, noticed an issue with building pool option and went to fix it as well #18
</commit_message>
<xml_diff>
--- a/data/save_board.xlsx
+++ b/data/save_board.xlsx
@@ -681,17 +681,17 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>MON</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>HSE</t>
+          <t>MON</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>FAC</t>
+          <t>MON</t>
         </is>
       </c>
       <c r="R3" s="1" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="W3" s="1" t="inlineStr">
         <is>
-          <t>FAC</t>
+          <t>MON</t>
         </is>
       </c>
       <c r="X3" s="1" t="inlineStr">
@@ -943,17 +943,17 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>HWY</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="Q5" s="1" t="inlineStr">
         <is>
-          <t>SHP</t>
+          <t>HWY</t>
         </is>
       </c>
       <c r="R5" s="1" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="W5" s="1" t="inlineStr">
         <is>
-          <t>HSE</t>
+          <t>HWY</t>
         </is>
       </c>
       <c r="X5" s="1" t="inlineStr">
@@ -1205,17 +1205,17 @@
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>PRK</t>
         </is>
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>PRK</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="Q7" s="1" t="inlineStr">
         <is>
-          <t>HSE</t>
+          <t>PRK</t>
         </is>
       </c>
       <c r="R7" s="1" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="W7" s="1" t="inlineStr">
         <is>
-          <t>FAC</t>
+          <t>PRK</t>
         </is>
       </c>
       <c r="X7" s="1" t="inlineStr">
@@ -1467,17 +1467,17 @@
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>MON</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="G9" s="1" t="inlineStr">
@@ -1497,17 +1497,17 @@
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>PRK</t>
         </is>
       </c>
       <c r="L9" s="1" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>n</t>
         </is>
       </c>
       <c r="M9" s="1" t="inlineStr">
@@ -1562,7 +1562,7 @@
       </c>
       <c r="W9" s="1" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>MON</t>
         </is>
       </c>
       <c r="X9" s="1" t="inlineStr">

</xml_diff>